<commit_message>
Update of nemo-only-list after fixing crashes in create-nemo-only-list.sh due to #482 & #481.
</commit_message>
<xml_diff>
--- a/ece2cmor3/scripts/create-nemo-only-list/nemo-only-list-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/scripts/create-nemo-only-list/nemo-only-list-cmpi6-requested-variables.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4769" uniqueCount="1560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4769" uniqueCount="1559">
   <si>
     <t>Table</t>
   </si>
@@ -259,7 +259,7 @@
     <t>longitude latitude time typesi</t>
   </si>
   <si>
-    <t>Sea-ice Area Percentage (Ocean Grid)</t>
+    <t>Sea-Ice Area Percentage (Ocean Grid)</t>
   </si>
   <si>
     <t>%</t>
@@ -268,7 +268,7 @@
     <t>Identified in the shaconemo (r274) seaIce ping file: iceconc_pct</t>
   </si>
   <si>
-    <t>Area fraction of grid cell covered by sea ice</t>
+    <t>Percentage of grid cell covered by sea ice</t>
   </si>
   <si>
     <t>C4MIP,CDRMIP,CFMIP,CMIP,CORDEX,DAMIP,DCPP,FAFMIP,GMMIP,GeoMIP,HighResMIP,LS3MIP,PAMIP,PMIP,RFMIP,SIMIP,VIACSAB</t>
@@ -280,7 +280,7 @@
     <t>sidconcdyn</t>
   </si>
   <si>
-    <t>Sea-ice Area Percentage Tendency Due to Dynamics</t>
+    <t>Sea-Ice Area Percentage Tendency Due to Dynamics</t>
   </si>
   <si>
     <t>s-1</t>
@@ -298,7 +298,7 @@
     <t>sidconcth</t>
   </si>
   <si>
-    <t>Sea-ice Area Percentage Tendency Due to Thermodynamics</t>
+    <t>Sea-Ice Area Percentage Tendency Due to Thermodynamics</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) seaIce ping file: afxthd</t>
@@ -742,7 +742,7 @@
     <t>Identified in the shaconemo (r274) seaIce ping file: iceconc_cat_pct_mv</t>
   </si>
   <si>
-    <t>Area fraction of grid cell covered by each ice-thickness category (vector with one entry for each thickness category starting from the thinnest category, netcdf file should use thickness bounds of the categories as third coordinate axis)</t>
+    <t>Percentage of grid cell covered by each ice-thickness category (vector with one entry for each thickness category starting from the thinnest category, netcdf file should use thickness bounds of the categories as third coordinate axis)</t>
   </si>
   <si>
     <t xml:space="preserve"> P3 (%) siitdconc : Area fraction of grid cell covered by each ice-thickness category (vector with one entry for each thickness category starting from the thinnest category, netcdf file should use thickness bounds of the categories as third coordinate axis) </t>
@@ -1306,7 +1306,7 @@
     <t>bfe</t>
   </si>
   <si>
-    <t>Mole Concentration of Particulate Organic Matter expressed as Iron in sea water</t>
+    <t>Mole Concentration of Particulate Organic Matter Expressed as Iron in Sea Water</t>
   </si>
   <si>
     <t>mol m-3</t>
@@ -1378,7 +1378,7 @@
     <t>bsi</t>
   </si>
   <si>
-    <t>Mole Concentration of Particulate Organic Matter Expressed as Silicon in sea water</t>
+    <t>Mole Concentration of Particulate Organic Matter Expressed as Silicon in Sea Water</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) ocnBgchem ping file: GSi_E3T</t>
@@ -1459,7 +1459,7 @@
     <t>cfc12</t>
   </si>
   <si>
-    <t>Mole Concentration of CFC12 in Sea water</t>
+    <t>Mole Concentration of CFC12 in Sea Water</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) ocean ping file: CFC12_E3T</t>
@@ -1477,7 +1477,7 @@
     <t>chl</t>
   </si>
   <si>
-    <t>Mass Concentration of Total Phytoplankton expressed as Chlorophyll in Sea Water</t>
+    <t>Mass Concentration of Total Phytoplankton Expressed as Chlorophyll in Sea Water</t>
   </si>
   <si>
     <t>kg m-3</t>
@@ -1498,7 +1498,7 @@
     <t>chldiat</t>
   </si>
   <si>
-    <t>Mass Concentration of Diatoms expressed as Chlorophyll in Sea Water</t>
+    <t>Mass Concentration of Diatoms Expressed as Chlorophyll in Sea Water</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) ocnBgchem ping file: DCHL_E3T</t>
@@ -1525,7 +1525,7 @@
     <t>chlmisc</t>
   </si>
   <si>
-    <t>Mass Concentration of Other Phytoplankton expressed as Chlorophyll in Sea Water</t>
+    <t>Mass Concentration of Other Phytoplankton Expressed as Chlorophyll in Sea Water</t>
   </si>
   <si>
     <t>Chlorophyll from additional phytoplankton component concentrations alone</t>
@@ -1549,7 +1549,7 @@
     <t>chlos</t>
   </si>
   <si>
-    <t>Surface Mass Concentration of Total Phytoplankton expressed as Chlorophyll in Sea Water</t>
+    <t>Surface Mass Concentration of Total Phytoplankton Expressed as Chlorophyll in Sea Water</t>
   </si>
   <si>
     <t>Sum of chlorophyll from all phytoplankton group concentrations at the sea surface.  In most models this is equal to chldiat+chlmisc, that is the sum of 'Diatom Chlorophyll Mass Concentration' plus 'Other Phytoplankton Chlorophyll Mass Concentration'</t>
@@ -1957,7 +1957,7 @@
     <t>fbddtdip</t>
   </si>
   <si>
-    <t>Rate of Change of Dissolved Inorganic Phosphorus due to Biological Activity</t>
+    <t>Rate of Change of Dissolved Inorganic Phosphorus Due to Biological Activity</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) ocnBgchem ping file: INTdtDIP</t>
@@ -1972,7 +1972,7 @@
     <t>fbddtdisi</t>
   </si>
   <si>
-    <t>Rate of Change of Dissolved Inorganic Silicon due to Biological Activity</t>
+    <t>Rate of Change of Dissolved Inorganic Silicon Due to Biological Activity</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) ocnBgchem ping file: INTdtSil</t>
@@ -3073,7 +3073,7 @@
     <t>phyfe</t>
   </si>
   <si>
-    <t>Mole Concentration of Total Phytoplankton expressed as Iron in sea water</t>
+    <t>Mole Concentration of Total Phytoplankton Expressed as Iron in Sea Water</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) ocnBgchem ping file: NFe_E3T</t>
@@ -3118,7 +3118,7 @@
     <t>physi</t>
   </si>
   <si>
-    <t>Mole Concentration of Total Phytoplankton expressed as Silicon in sea water</t>
+    <t>Mole Concentration of Total Phytoplankton Expressed as Silicon in Sea Water</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) ocnBgchem ping file: DSi_E3T</t>
@@ -3241,7 +3241,7 @@
     <t>sf6</t>
   </si>
   <si>
-    <t>Mole Concentration of SF6 in sea water</t>
+    <t>Mole Concentration of SF6 in Sea Water</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) ocean ping file: SF6_E3T</t>
@@ -4024,7 +4024,7 @@
     <t>ocontempdiff</t>
   </si>
   <si>
-    <t>Tendency of Sea Water Conservative Temperature Expressed as Heat Content due to Parameterized Dianeutral Mixing</t>
+    <t>Tendency of Sea Water Conservative Temperature Expressed as Heat Content Due to Parameterized Dianeutral Mixing</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) ocean ping file: ttrd_zdfp_e3t</t>
@@ -4099,7 +4099,7 @@
     <t>osaltdiff</t>
   </si>
   <si>
-    <t>Tendency of Sea water Salinity Expressed as Salt Content Due to Parameterized Dianeutral Mixing</t>
+    <t>Tendency of Sea Water Salinity Expressed as Salt Content Due to Parameterized Dianeutral Mixing</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) ocean ping file: strd_zdfp_e3t</t>
@@ -4114,7 +4114,7 @@
     <t>osaltpadvect</t>
   </si>
   <si>
-    <t>Tendency of Sea water Salinity Expressed as Salt Content Due to Parameterized Eddy Advection</t>
+    <t>Tendency of Sea Water Salinity Expressed as Salt Content Due to Parameterized Eddy Advection</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) ocean ping file: strd_eivad_e3t</t>
@@ -4129,7 +4129,7 @@
     <t>osaltpmdiff</t>
   </si>
   <si>
-    <t>Tendency of Sea water Salinity Expressed as Salt Content Due to Parameterized Mesoscale Diffusion</t>
+    <t>Tendency of Sea Water Salinity Expressed as Salt Content Due to Parameterized Mesoscale Diffusion</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) ocean ping file: strd_iso_e3t</t>
@@ -4159,7 +4159,7 @@
     <t>osalttend</t>
   </si>
   <si>
-    <t>Tendency of Sea water Salinity Expressed as Salt Content</t>
+    <t>Tendency of Sea Water Salinity Expressed as Salt Content</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) ocean ping file: strd_tot_e3t</t>
@@ -4468,7 +4468,7 @@
     <t>longitude latitude time2</t>
   </si>
   <si>
-    <t>Ocean Tracer Diffusivity due to Parameterized Mesoscale Advection</t>
+    <t>Ocean Tracer Diffusivity Due to Parameterized Mesoscale Advection</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) ocean ping file: aht2d_eiv</t>
@@ -4594,7 +4594,7 @@
     <t>tnkebto2d</t>
   </si>
   <si>
-    <t>Tendency of Ocean Eddy Kinetic Energy Content due to Parameterized Eddy Advection</t>
+    <t>Tendency of Ocean Eddy Kinetic Energy Content Due to Parameterized Eddy Advection</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) ocean ping file: eketrd_eiv</t>
@@ -4675,16 +4675,13 @@
     <t>sftof</t>
   </si>
   <si>
-    <t>longitude latitude typesea</t>
-  </si>
-  <si>
     <t>Sea Area Percentage</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) ocean ping file: iceconc_pct</t>
   </si>
   <si>
-    <t>This is the area fraction at the ocean surface.</t>
+    <t>Percentage of horizontal area occupied by ocean.</t>
   </si>
   <si>
     <t xml:space="preserve"> P1 (%) sea_area_fraction : This is the area fraction at the ocean surface. **** NEMO-RD: variable already provided in ping_seaIce under name siconc - we decide to keep it here as well </t>
@@ -21536,10 +21533,10 @@
         <v>28</v>
       </c>
       <c r="D377" t="s">
+        <v>1533</v>
+      </c>
+      <c r="E377" t="s">
         <v>1553</v>
-      </c>
-      <c r="E377" t="s">
-        <v>1554</v>
       </c>
       <c r="F377" t="s">
         <v>82</v>
@@ -21549,13 +21546,13 @@
         <v>0</v>
       </c>
       <c r="H377" t="s">
+        <v>1554</v>
+      </c>
+      <c r="I377" t="s">
+        <v>21</v>
+      </c>
+      <c r="J377" t="s">
         <v>1555</v>
-      </c>
-      <c r="I377" t="s">
-        <v>21</v>
-      </c>
-      <c r="J377" t="s">
-        <v>1556</v>
       </c>
       <c r="K377" t="s">
         <v>1537</v>
@@ -21567,7 +21564,7 @@
         <v>82</v>
       </c>
       <c r="N377" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="378" spans="1:14">
@@ -21603,7 +21600,7 @@
         <v>1164</v>
       </c>
       <c r="K378" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="L378" t="s">
         <v>24</v>
@@ -21617,7 +21614,7 @@
     </row>
     <row r="380" spans="1:14">
       <c r="A380" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="B380" t="s">
         <v>919</v>
@@ -21662,7 +21659,7 @@
     </row>
     <row r="381" spans="1:14">
       <c r="A381" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="B381" t="s">
         <v>1440</v>

</xml_diff>

<commit_message>
Update the nemo only list #526.
</commit_message>
<xml_diff>
--- a/ece2cmor3/scripts/create-nemo-only-list/nemo-only-list-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/scripts/create-nemo-only-list/nemo-only-list-cmpi6-requested-variables.xlsx
@@ -2020,7 +2020,7 @@
     <t>fgco2</t>
   </si>
   <si>
-    <t>Surface Downward Flux of Total CO2</t>
+    <t>Surface Downward Mass Flux of Carbon as CO2 [kgC m-2 s-1]</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) ocnBgchem ping file: Cflx</t>
@@ -3445,7 +3445,7 @@
     <t>tauuo</t>
   </si>
   <si>
-    <t>Surface Downward X Stress</t>
+    <t>Sea Water Surface Downward X Stress</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) ocean ping file: utau</t>
@@ -3460,7 +3460,7 @@
     <t>tauvo</t>
   </si>
   <si>
-    <t>Surface Downward Y Stress</t>
+    <t>Sea Water Surface Downward Y Stress</t>
   </si>
   <si>
     <t>Identified in the shaconemo (r274) ocean ping file: vtau</t>
@@ -3658,7 +3658,7 @@
     <t>Identified in the shaconemo (r274) ocean ping file: erp</t>
   </si>
   <si>
-    <t>Positive flux implies correction adds water to ocean.</t>
+    <t>Computed as the water flux into the ocean due to flux correction divided by the area of the ocean portion of the grid cell.</t>
   </si>
   <si>
     <t xml:space="preserve"> P1 (kg m-2 s-1) water_flux_correction : Positive flux implies correction adds water to ocean. </t>
@@ -3673,7 +3673,7 @@
     <t>Identified in the shaconemo (r274) ocean ping file: empmr</t>
   </si>
   <si>
-    <t>computed as the water  flux into the ocean divided by the area of the ocean portion of the grid cell.  This is the sum of the next two variables in this table.</t>
+    <t>Computed as the water flux into the ocean divided by the area of the ocean portion of the grid cell. This is the sum *wfonocorr* and *wfcorr*.</t>
   </si>
   <si>
     <t xml:space="preserve"> P1 (kg m-2 s-1) water_flux_into_sea_water : computed as the water  flux into the ocean divided by the area of the ocean portion of the grid cell.  This is the sum of the next two variables in this table.  </t>
@@ -3685,7 +3685,7 @@
     <t>Water Flux into Sea Water Without Flux Correction</t>
   </si>
   <si>
-    <t>computed as the water  flux (without flux correction) into the ocean divided by the area of the ocean portion of the grid cell.</t>
+    <t>Computed as the water flux (without flux correction) into the ocean divided by the area of the ocean portion of the grid cell.</t>
   </si>
   <si>
     <t xml:space="preserve"> P1 (kg m-2 s-1) water_flux_into_sea_water_without_flux_correction : computed as the water  flux (without flux correction) into the ocean divided by the area of the ocean portion of the grid cell. *** NEMO-RD : TODO in field_ocean, empmr is defined as water flux out of sea ice and sea water. Is sea ice really taken into here? If no, correct description in field. If yes, this input is wrong here. </t>

</xml_diff>